<commit_message>
Added timeout to redirect from create new listing/listing edit
</commit_message>
<xml_diff>
--- a/DTT-Test-Hour-Log.xlsx
+++ b/DTT-Test-Hour-Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaniekvandermaarel/Documents/DTT stage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{173D51CE-4E2F-4F40-9157-58C916CA122A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1585CE28-FFC7-46C3-A134-8716A0CA4A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,6 +197,7 @@
   <si>
     <t>Removed the ability for users to edit a page when a specific url is typed into the browser.
 Fixed an issue where page redirection broke when a number without decimal speration was given.
+Added a timeout to page redirect to allow image to be uploaded to API before user enters details page.
 Cleaned up my code.</t>
   </si>
   <si>
@@ -1812,7 +1813,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -2003,12 +2004,12 @@
       <c r="E12" s="3"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="51" customHeight="1">
+    <row r="13" spans="1:6" ht="75.75" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="18">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C13" s="19">
         <v>44477</v>
@@ -2153,7 +2154,7 @@
       </c>
       <c r="B30" s="15">
         <f>SUM(B4:B28)</f>
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>

</xml_diff>